<commit_message>
tak-4 has been completed
</commit_message>
<xml_diff>
--- a/European_Coaching/day_4/excel/task-2.xlsx
+++ b/European_Coaching/day_4/excel/task-2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,9 +15,41 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>RATE OF BIKE</t>
+  </si>
+  <si>
+    <t>DOWN PAYMENT</t>
+  </si>
+  <si>
+    <t>LAON AMOUNT</t>
+  </si>
+  <si>
+    <t>RATE OF INTEREST</t>
+  </si>
+  <si>
+    <t>DURATION</t>
+  </si>
+  <si>
+    <t>INSTALLMENT</t>
+  </si>
+  <si>
+    <t>TOTAL AMOUNT TOBE PAID</t>
+  </si>
+  <si>
+    <t>TOTAL INTEREST PAID</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;₹&quot;\ #,##0.00;[Red]&quot;₹&quot;\ \-#,##0.00"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,14 +78,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +382,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>62500</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>38500</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1763.28</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2">
+        <v>42318.77</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3818.77</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>